<commit_message>
Reverting impl of templates
</commit_message>
<xml_diff>
--- a/src/main/webapp/templates/commissionStatementTemplate.xlsx
+++ b/src/main/webapp/templates/commissionStatementTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace_phase3\Product-2.10.3.0-build1790\WebContent\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10676922\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C624F8-E93B-47E6-8F38-378D45FB5060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20595" windowHeight="7860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Page" sheetId="1" r:id="rId1"/>
@@ -510,7 +511,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1074,19 +1075,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>50938</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>98563</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>153194</xdr:rowOff>
+      <xdr:rowOff>57944</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1099,7 +1106,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="279538" y="200025"/>
+          <a:off x="327163" y="104775"/>
           <a:ext cx="587237" cy="562769"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1129,7 +1136,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="E:\workspace_phase3\Product-2.10.3.0-build1790\WebContent\images\bmicLogo2.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="E:\workspace_phase3\Product-2.10.3.0-build1790\WebContent\images\bmicLogo2.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1189,7 +1202,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1232,7 +1251,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1520,11 +1545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BE24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2051,7 +2076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2341,7 +2366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2353,7 +2378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:J45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2792,7 +2817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
commission statement updated template
</commit_message>
<xml_diff>
--- a/src/main/webapp/templates/commissionStatementTemplate.xlsx
+++ b/src/main/webapp/templates/commissionStatementTemplate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10676922\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace_phase3\Product-2.10.3.0-build1790\WebContent\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F577D8-4E12-4FDE-9162-76B83C6865F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20595" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Page" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="159">
   <si>
     <t>AGENCY DETAILS</t>
   </si>
@@ -506,15 +505,12 @@
   </si>
   <si>
     <t>:Producer_Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUILDERS MUTUAL INSURANCE </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1078,25 +1074,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>98564</xdr:colOff>
+      <xdr:colOff>3314</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>625338</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>451402</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>105568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1109,8 +1099,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="327164" y="104775"/>
-          <a:ext cx="526774" cy="504825"/>
+          <a:off x="231914" y="123825"/>
+          <a:ext cx="448088" cy="429418"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1127,60 +1117,37 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>41636</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
+      <xdr:colOff>671379</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>134520</xdr:rowOff>
+      <xdr:rowOff>132642</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="E:\workspace_phase3\Product-2.10.3.0-build1790\WebContent\images\bmicLogo2.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="346436" y="133350"/>
-          <a:ext cx="663214" cy="629820"/>
+          <a:off x="323850" y="133350"/>
+          <a:ext cx="652329" cy="627942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1193,25 +1160,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>684558</xdr:colOff>
+      <xdr:colOff>652329</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:rowOff>113592</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1224,8 +1185,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171451" y="152401"/>
-          <a:ext cx="655982" cy="628650"/>
+          <a:off x="142875" y="142875"/>
+          <a:ext cx="652329" cy="627942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1242,25 +1203,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>134245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:colOff>685801</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>124222</xdr:rowOff>
+      <xdr:rowOff>77343</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1273,8 +1228,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="257175" y="161925"/>
-          <a:ext cx="676275" cy="648097"/>
+          <a:off x="247650" y="134245"/>
+          <a:ext cx="657226" cy="628898"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1548,11 +1503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1586,7 +1541,7 @@
     <row r="3" spans="1:51" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -2079,10 +2034,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +2324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2381,11 +2336,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2820,11 +2775,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>